<commit_message>
added additional contest results and payout data
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="821"/>
+    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
     <sheet name="$3_payout_structure_week1.csv" sheetId="4" r:id="rId2"/>
     <sheet name="$3_payout_structure_week2.csv" sheetId="5" r:id="rId3"/>
     <sheet name="$3_payout_structure_week3.csv" sheetId="2" r:id="rId4"/>
-    <sheet name="$20_payout_structure_week3.csv" sheetId="6" r:id="rId5"/>
+    <sheet name="$5_payout_structure_week3.csv" sheetId="9" r:id="rId5"/>
+    <sheet name="$9_payout_structure_week3.csv" sheetId="8" r:id="rId6"/>
+    <sheet name="$20_payout_structure_week3.csv" sheetId="6" r:id="rId7"/>
+    <sheet name="$333_payout_structure_week3.csv" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>1st</t>
   </si>
@@ -50,12 +53,6 @@
   </si>
   <si>
     <t>11th - 15th</t>
-  </si>
-  <si>
-    <t>26th - 35th</t>
-  </si>
-  <si>
-    <t>36th - 50th</t>
   </si>
   <si>
     <t>51st - 75th</t>
@@ -100,25 +97,7 @@
     <t>401st - 500th</t>
   </si>
   <si>
-    <t>501st - 700th</t>
-  </si>
-  <si>
-    <t>701st - 1000th</t>
-  </si>
-  <si>
     <t>1501st - 2500th</t>
-  </si>
-  <si>
-    <t>2501st - 3500th</t>
-  </si>
-  <si>
-    <t>3501st - 5000th</t>
-  </si>
-  <si>
-    <t>5001st - 8000th</t>
-  </si>
-  <si>
-    <t>8001st - 14000th</t>
   </si>
   <si>
     <t>14001st - 26000th</t>
@@ -128,6 +107,30 @@
   </si>
   <si>
     <t>44002nd - 70623rd</t>
+  </si>
+  <si>
+    <t>26th - 30th</t>
+  </si>
+  <si>
+    <t>31st - 40th</t>
+  </si>
+  <si>
+    <t>41st - 50th</t>
+  </si>
+  <si>
+    <t>501st - 750th</t>
+  </si>
+  <si>
+    <t>751st - 1000th</t>
+  </si>
+  <si>
+    <t>2501st - 5000th</t>
+  </si>
+  <si>
+    <t>5001st - 9625th</t>
+  </si>
+  <si>
+    <t>9626th - 18750th</t>
   </si>
 </sst>
 </file>
@@ -179,8 +182,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +226,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -223,6 +236,11 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -232,6 +250,11 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -578,19 +601,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -598,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1000000</v>
+        <v>15000</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -608,7 +631,7 @@
       </c>
       <c r="F2" s="3">
         <f>B2</f>
-        <v>1000000</v>
+        <v>15000</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -617,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>200000</v>
+        <v>10000</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:E7" si="0">D2+1</f>
@@ -629,7 +652,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F34" si="1">B3</f>
-        <v>200000</v>
+        <v>10000</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -638,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -650,7 +673,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -659,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -671,7 +694,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -680,7 +703,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>25000</v>
+        <v>3500</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -692,7 +715,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>3500</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -701,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>15000</v>
+        <v>2500</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -713,7 +736,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>2500</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -722,7 +745,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ref="D8:D34" si="2">LEFT(A8,FIND(" ",A8)-3)</f>
@@ -734,7 +757,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -743,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="2"/>
@@ -755,7 +778,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -764,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
@@ -776,16 +799,16 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>4000</v>
+        <v>750</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
@@ -797,16 +820,16 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>750</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -818,16 +841,16 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
@@ -835,297 +858,297 @@
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1">
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
-        <v>750</v>
+        <v>250</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>250</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>300</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>301</v>
+        <v>201</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>75</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>501</v>
+        <v>401</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>701</v>
+        <v>501</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1001</v>
+        <v>751</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1501</v>
+        <v>1001</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>2501</v>
+        <v>1501</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>3501</v>
+        <v>2501</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1133,16 +1156,16 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1150,38 +1173,38 @@
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>8000</v>
+        <v>9625</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>8001</v>
+        <v>9626</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>14000</v>
+        <v>18750</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1">
         <v>40</v>
@@ -1202,7 +1225,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1">
         <v>34</v>
@@ -1223,7 +1246,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1">
         <v>30</v>
@@ -1309,19 +1332,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1757,20 +1782,20 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2150,21 +2175,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2542,6 +2565,662 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4">
+        <v>76</v>
+      </c>
+      <c r="B17" s="4">
+        <v>100</v>
+      </c>
+      <c r="C17" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>101</v>
+      </c>
+      <c r="B18" s="4">
+        <v>150</v>
+      </c>
+      <c r="C18" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
+        <v>151</v>
+      </c>
+      <c r="B19" s="4">
+        <v>200</v>
+      </c>
+      <c r="C19" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4">
+        <v>201</v>
+      </c>
+      <c r="B20" s="4">
+        <v>300</v>
+      </c>
+      <c r="C20" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4">
+        <v>301</v>
+      </c>
+      <c r="B21" s="4">
+        <v>400</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4">
+        <v>401</v>
+      </c>
+      <c r="B22" s="4">
+        <v>500</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4">
+        <v>501</v>
+      </c>
+      <c r="B23" s="4">
+        <v>750</v>
+      </c>
+      <c r="C23" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4">
+        <v>751</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4">
+        <v>1001</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1500</v>
+      </c>
+      <c r="C25" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4">
+        <v>1501</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2500</v>
+      </c>
+      <c r="C26" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4">
+        <v>2501</v>
+      </c>
+      <c r="B27" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C27" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4">
+        <v>5001</v>
+      </c>
+      <c r="B28" s="4">
+        <v>9625</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4">
+        <v>9626</v>
+      </c>
+      <c r="B29" s="4">
+        <v>18750</v>
+      </c>
+      <c r="C29" s="3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4">
+        <v>75</v>
+      </c>
+      <c r="C14" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4">
+        <v>76</v>
+      </c>
+      <c r="B15" s="4">
+        <v>125</v>
+      </c>
+      <c r="C15" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>126</v>
+      </c>
+      <c r="B16" s="4">
+        <v>200</v>
+      </c>
+      <c r="C16" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4">
+        <v>201</v>
+      </c>
+      <c r="B17" s="4">
+        <v>300</v>
+      </c>
+      <c r="C17" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>301</v>
+      </c>
+      <c r="B18" s="4">
+        <v>400</v>
+      </c>
+      <c r="C18" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
+        <v>401</v>
+      </c>
+      <c r="B19" s="4">
+        <v>500</v>
+      </c>
+      <c r="C19" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4">
+        <v>501</v>
+      </c>
+      <c r="B20" s="4">
+        <v>650</v>
+      </c>
+      <c r="C20" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4">
+        <v>651</v>
+      </c>
+      <c r="B21" s="4">
+        <v>900</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4">
+        <v>901</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1400</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4">
+        <v>1401</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2200</v>
+      </c>
+      <c r="C23" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4">
+        <v>2201</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3200</v>
+      </c>
+      <c r="C24" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4">
+        <v>3201</v>
+      </c>
+      <c r="B25" s="4">
+        <v>5200</v>
+      </c>
+      <c r="C25" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4">
+        <v>5201</v>
+      </c>
+      <c r="B26" s="4">
+        <v>9200</v>
+      </c>
+      <c r="C26" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4">
+        <v>9201</v>
+      </c>
+      <c r="B27" s="4">
+        <v>15850</v>
+      </c>
+      <c r="C27" s="3">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2552,13 +3231,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2900,6 +3579,235 @@
       </c>
       <c r="C32" s="3">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4">
+        <v>75</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4">
+        <v>76</v>
+      </c>
+      <c r="B15" s="4">
+        <v>100</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>101</v>
+      </c>
+      <c r="B16" s="4">
+        <v>150</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4">
+        <v>151</v>
+      </c>
+      <c r="B17" s="4">
+        <v>270</v>
+      </c>
+      <c r="C17" s="3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>271</v>
+      </c>
+      <c r="B18" s="4">
+        <v>520</v>
+      </c>
+      <c r="C18" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
+        <v>521</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="3">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 8 $3 results and payout structure
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="$20_payout_structure_week3.csv" sheetId="6" r:id="rId7"/>
     <sheet name="$333_payout_structure_week3.csv" sheetId="7" r:id="rId8"/>
     <sheet name="$3_payout_structure_week6.csv" sheetId="10" r:id="rId9"/>
+    <sheet name="$3_payout_structure_week8" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>1st</t>
   </si>
@@ -189,8 +190,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -236,7 +241,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -252,6 +257,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -267,6 +274,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -598,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:F34"/>
     </sheetView>
   </sheetViews>
@@ -1342,6 +1351,400 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>201</v>
+      </c>
+      <c r="B18" s="5">
+        <v>250</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>251</v>
+      </c>
+      <c r="B19" s="5">
+        <v>350</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>351</v>
+      </c>
+      <c r="B20" s="5">
+        <v>450</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>451</v>
+      </c>
+      <c r="B21" s="5">
+        <v>700</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>701</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>1001</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1501</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2501</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>4001</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6500</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>6501</v>
+      </c>
+      <c r="B27" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>10001</v>
+      </c>
+      <c r="B28" s="5">
+        <v>15000</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>15001</v>
+      </c>
+      <c r="B29" s="5">
+        <v>22000</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5">
+        <v>22001</v>
+      </c>
+      <c r="B30" s="5">
+        <v>32000</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5">
+        <v>32001</v>
+      </c>
+      <c r="B31" s="5">
+        <v>45000</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5">
+        <v>45001</v>
+      </c>
+      <c r="B32" s="5">
+        <v>65000</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5">
+        <v>65001</v>
+      </c>
+      <c r="B33" s="5">
+        <v>100000</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5">
+        <v>100001</v>
+      </c>
+      <c r="B34" s="5">
+        <v>161100</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3846,8 +4249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
week 10 payout structure
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="$333_payout_structure_week3.csv" sheetId="7" r:id="rId8"/>
     <sheet name="$3_payout_structure_week6.csv" sheetId="10" r:id="rId9"/>
     <sheet name="$3_payout_structure_week8" sheetId="11" r:id="rId10"/>
+    <sheet name="$4_payout_structure_week10" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>1st</t>
   </si>
@@ -81,12 +82,6 @@
     <t>Place_hi</t>
   </si>
   <si>
-    <t>1001st - 1500th</t>
-  </si>
-  <si>
-    <t>1501st - 2500th</t>
-  </si>
-  <si>
     <t>16th - 25th</t>
   </si>
   <si>
@@ -96,49 +91,49 @@
     <t>36th - 50th</t>
   </si>
   <si>
-    <t>201st - 250th</t>
+    <t>201st - 300th</t>
   </si>
   <si>
-    <t>251st - 350th</t>
+    <t>301st - 500th</t>
   </si>
   <si>
-    <t>351st - 450th</t>
+    <t>501st - 750th</t>
   </si>
   <si>
-    <t>451st - 700th</t>
+    <t>751st - 1250th</t>
   </si>
   <si>
-    <t>701st - 1000th</t>
+    <t>1251st - 2000th</t>
   </si>
   <si>
-    <t>2501st - 4000th</t>
+    <t>2001st - 3000th</t>
   </si>
   <si>
-    <t>4001st - 6500th</t>
+    <t>3001st - 4000th</t>
   </si>
   <si>
-    <t>6501st - 10000th</t>
+    <t>4001st - 6000th</t>
   </si>
   <si>
-    <t>10001st - 15000th</t>
+    <t>6001st - 9000th</t>
   </si>
   <si>
-    <t>15001st - 22000th</t>
+    <t>9001st - 13000th</t>
   </si>
   <si>
-    <t>22001st - 32000th</t>
+    <t>13001st - 20000th</t>
   </si>
   <si>
-    <t>32001st - 45000th</t>
+    <t>20001st - 30000th</t>
   </si>
   <si>
-    <t>45001st - 65000th</t>
+    <t>30001st - 50000th</t>
   </si>
   <si>
-    <t>65001st - 100000th</t>
+    <t>50001st - 88000th</t>
   </si>
   <si>
-    <t>100001st - 161100th</t>
+    <t>88001st - 160875th</t>
   </si>
 </sst>
 </file>
@@ -154,6 +149,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,8 +186,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,7 +241,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -259,6 +259,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -276,6 +278,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D1:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -642,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -652,7 +656,7 @@
       </c>
       <c r="F2" s="3">
         <f>B2</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -661,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:E7" si="0">D2+1</f>
@@ -673,7 +677,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F34" si="1">B3</f>
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -682,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -694,7 +698,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -703,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -715,7 +719,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -724,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>7500</v>
+        <v>12500</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -736,7 +740,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>12500</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -745,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -757,7 +761,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -766,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ref="D8:D34" si="2">LEFT(A8,FIND(" ",A8)-3)</f>
@@ -778,7 +782,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -787,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="2"/>
@@ -799,7 +803,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -808,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
@@ -820,16 +824,16 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
@@ -841,16 +845,16 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -862,16 +866,16 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
@@ -883,7 +887,7 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -892,7 +896,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>400</v>
+        <v>750</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
@@ -904,7 +908,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>750</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -913,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -925,7 +929,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -934,7 +938,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
@@ -946,7 +950,7 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -955,7 +959,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
@@ -967,16 +971,16 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="2"/>
@@ -984,137 +988,137 @@
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>351</v>
+        <v>501</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>451</v>
+        <v>751</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>700</v>
+        <v>1250</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>701</v>
+        <v>1251</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1001</v>
+        <v>2001</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1501</v>
+        <v>3001</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1123,19 +1127,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>2501</v>
+        <v>4001</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -1144,19 +1148,19 @@
         <v>28</v>
       </c>
       <c r="B26" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>4001</v>
+        <v>6001</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>6500</v>
+        <v>9000</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I26" s="1"/>
     </row>
@@ -1165,19 +1169,19 @@
         <v>29</v>
       </c>
       <c r="B27" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>6501</v>
+        <v>9001</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -1186,19 +1190,19 @@
         <v>30</v>
       </c>
       <c r="B28" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>10001</v>
+        <v>13001</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I28" s="1"/>
     </row>
@@ -1207,19 +1211,19 @@
         <v>31</v>
       </c>
       <c r="B29" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>15001</v>
+        <v>20001</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>22000</v>
+        <v>30000</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -1228,19 +1232,19 @@
         <v>32</v>
       </c>
       <c r="B30" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>22001</v>
+        <v>30001</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>32000</v>
+        <v>50000</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -1253,11 +1257,11 @@
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>32001</v>
+        <v>50001</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>45000</v>
+        <v>88000</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
@@ -1270,81 +1274,71 @@
         <v>34</v>
       </c>
       <c r="B32" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>45001</v>
+        <v>88001</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>65000</v>
+        <v>160875</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="1">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="str">
+    <row r="33" spans="2:9">
+      <c r="B33" s="1"/>
+      <c r="D33" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>65001</v>
-      </c>
-      <c r="E33" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E33" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>100000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="1">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="str">
+    <row r="34" spans="2:9">
+      <c r="B34" s="1"/>
+      <c r="D34" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>100001</v>
-      </c>
-      <c r="E34" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E34" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>161100</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="2:9">
       <c r="B35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="2:9">
       <c r="B36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="2:9">
       <c r="B37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="2:9">
       <c r="B38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="2:9">
       <c r="B39" s="1"/>
       <c r="I39" s="1"/>
     </row>
@@ -1363,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1741,6 +1735,378 @@
       </c>
       <c r="C34">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>201</v>
+      </c>
+      <c r="B18" s="5">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>301</v>
+      </c>
+      <c r="B19" s="5">
+        <v>500</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>501</v>
+      </c>
+      <c r="B20" s="5">
+        <v>750</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>751</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1250</v>
+      </c>
+      <c r="C21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>1251</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2000</v>
+      </c>
+      <c r="C22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>3001</v>
+      </c>
+      <c r="B24" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>4001</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6000</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>6001</v>
+      </c>
+      <c r="B26" s="5">
+        <v>9000</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>9001</v>
+      </c>
+      <c r="B27" s="5">
+        <v>13000</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>13001</v>
+      </c>
+      <c r="B28" s="5">
+        <v>20000</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>20001</v>
+      </c>
+      <c r="B29" s="5">
+        <v>30000</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5">
+        <v>30001</v>
+      </c>
+      <c r="B30" s="5">
+        <v>50000</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5">
+        <v>50001</v>
+      </c>
+      <c r="B31" s="5">
+        <v>88000</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5">
+        <v>88001</v>
+      </c>
+      <c r="B32" s="5">
+        <v>160875</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added thursday game stuff
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="$3_payout_structure_week6.csv" sheetId="10" r:id="rId9"/>
     <sheet name="$3_payout_structure_week8" sheetId="11" r:id="rId10"/>
     <sheet name="$4_payout_structure_week10" sheetId="12" r:id="rId11"/>
+    <sheet name="$27_payout_structure_week15_thu" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>1st</t>
   </si>
@@ -55,21 +56,6 @@
     <t>9th - 10th</t>
   </si>
   <si>
-    <t>11th - 15th</t>
-  </si>
-  <si>
-    <t>51st - 75th</t>
-  </si>
-  <si>
-    <t>76th - 100th</t>
-  </si>
-  <si>
-    <t>101st - 150th</t>
-  </si>
-  <si>
-    <t>151st - 200th</t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
@@ -82,58 +68,34 @@
     <t>Place_hi</t>
   </si>
   <si>
-    <t>16th - 25th</t>
+    <t>11th - 13th</t>
   </si>
   <si>
-    <t>26th - 35th</t>
+    <t>14th - 18th</t>
   </si>
   <si>
-    <t>36th - 50th</t>
+    <t>19th - 25th</t>
   </si>
   <si>
-    <t>201st - 300th</t>
+    <t>26th - 37th</t>
   </si>
   <si>
-    <t>301st - 500th</t>
+    <t>38th - 65th</t>
   </si>
   <si>
-    <t>501st - 750th</t>
+    <t>66th - 115th</t>
   </si>
   <si>
-    <t>751st - 1250th</t>
+    <t>116th - 190th</t>
   </si>
   <si>
-    <t>1251st - 2000th</t>
+    <t>191st - 305th</t>
   </si>
   <si>
-    <t>2001st - 3000th</t>
+    <t>306th - 465th</t>
   </si>
   <si>
-    <t>3001st - 4000th</t>
-  </si>
-  <si>
-    <t>4001st - 6000th</t>
-  </si>
-  <si>
-    <t>6001st - 9000th</t>
-  </si>
-  <si>
-    <t>9001st - 13000th</t>
-  </si>
-  <si>
-    <t>13001st - 20000th</t>
-  </si>
-  <si>
-    <t>20001st - 30000th</t>
-  </si>
-  <si>
-    <t>30001st - 50000th</t>
-  </si>
-  <si>
-    <t>50001st - 88000th</t>
-  </si>
-  <si>
-    <t>88001st - 160875th</t>
+    <t>466th - 752nd</t>
   </si>
 </sst>
 </file>
@@ -186,8 +148,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,7 +205,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -261,6 +225,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -280,6 +245,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,7 +578,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D1:F32"/>
+      <selection activeCell="F19" sqref="D1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,19 +592,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -646,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>100000</v>
+        <v>5000</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -656,7 +622,7 @@
       </c>
       <c r="F2" s="3">
         <f>B2</f>
-        <v>100000</v>
+        <v>5000</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -665,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>50000</v>
+        <v>3000</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:E7" si="0">D2+1</f>
@@ -677,7 +643,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F34" si="1">B3</f>
-        <v>50000</v>
+        <v>3000</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -686,7 +652,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -698,7 +664,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -707,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -719,7 +685,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -728,7 +694,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>12500</v>
+        <v>1500</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -740,7 +706,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>12500</v>
+        <v>1500</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -749,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -761,7 +727,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -770,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>7500</v>
+        <v>750</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ref="D8:D34" si="2">LEFT(A8,FIND(" ",A8)-3)</f>
@@ -782,7 +748,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>750</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -791,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>5000</v>
+        <v>550</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="2"/>
@@ -803,16 +769,16 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>550</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>3000</v>
+        <v>400</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
@@ -820,158 +786,158 @@
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>400</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>1500</v>
+        <v>200</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>200</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>750</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>125</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>300</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>305</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>70</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -980,19 +946,19 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>201</v>
+        <v>306</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>465</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1001,292 +967,227 @@
         <v>21</v>
       </c>
       <c r="B19" s="1">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>301</v>
-      </c>
-      <c r="E19" s="2" t="str">
+        <v>466</v>
+      </c>
+      <c r="E19" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="1">
-        <v>100</v>
-      </c>
-      <c r="D20" s="2" t="str">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>501</v>
-      </c>
-      <c r="E20" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>750</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="1">
-        <v>80</v>
-      </c>
-      <c r="D21" s="2" t="str">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>751</v>
-      </c>
-      <c r="E21" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E21" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>1250</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1">
-        <v>60</v>
-      </c>
-      <c r="D22" s="2" t="str">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>1251</v>
-      </c>
-      <c r="E22" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E22" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="1">
-        <v>50</v>
-      </c>
-      <c r="D23" s="2" t="str">
+      <c r="B23" s="1"/>
+      <c r="D23" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>2001</v>
-      </c>
-      <c r="E23" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E23" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="1">
-        <v>40</v>
-      </c>
-      <c r="D24" s="2" t="str">
+      <c r="B24" s="1"/>
+      <c r="D24" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>3001</v>
-      </c>
-      <c r="E24" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E24" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="1">
-        <v>30</v>
-      </c>
-      <c r="D25" s="2" t="str">
+      <c r="B25" s="1"/>
+      <c r="D25" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>4001</v>
-      </c>
-      <c r="E25" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E25" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="1">
-        <v>25</v>
-      </c>
-      <c r="D26" s="2" t="str">
+      <c r="B26" s="1"/>
+      <c r="D26" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>6001</v>
-      </c>
-      <c r="E26" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E26" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>9000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="1">
-        <v>20</v>
-      </c>
-      <c r="D27" s="2" t="str">
+      <c r="B27" s="1"/>
+      <c r="D27" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>9001</v>
-      </c>
-      <c r="E27" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E27" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>13000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="1">
-        <v>15</v>
-      </c>
-      <c r="D28" s="2" t="str">
+      <c r="B28" s="1"/>
+      <c r="D28" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>13001</v>
-      </c>
-      <c r="E28" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E28" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>20000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2" t="str">
+      <c r="B29" s="1"/>
+      <c r="D29" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>20001</v>
-      </c>
-      <c r="E29" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E29" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>30000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="1">
-        <v>10</v>
-      </c>
-      <c r="D30" s="2" t="str">
+      <c r="B30" s="1"/>
+      <c r="D30" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>30001</v>
-      </c>
-      <c r="E30" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E30" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>50000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="1">
-        <v>8</v>
-      </c>
-      <c r="D31" s="2" t="str">
+      <c r="B31" s="1"/>
+      <c r="D31" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>50001</v>
-      </c>
-      <c r="E31" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E31" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>88000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="str">
+      <c r="B32" s="1"/>
+      <c r="D32" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>88001</v>
-      </c>
-      <c r="E32" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E32" s="2" t="e">
         <f t="shared" si="3"/>
-        <v>160875</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -1365,13 +1266,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1751,21 +1652,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2107,6 +2008,235 @@
       </c>
       <c r="C32">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5">
+        <v>37</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5">
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5">
+        <v>115</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>116</v>
+      </c>
+      <c r="B16" s="5">
+        <v>190</v>
+      </c>
+      <c r="C16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>191</v>
+      </c>
+      <c r="B17" s="5">
+        <v>305</v>
+      </c>
+      <c r="C17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>306</v>
+      </c>
+      <c r="B18" s="5">
+        <v>465</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>466</v>
+      </c>
+      <c r="B19">
+        <v>752</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2131,13 +2261,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2580,13 +2710,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2972,13 +3102,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3366,13 +3496,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3705,13 +3835,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4022,13 +4152,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4394,13 +4524,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4623,13 +4753,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
week 16 contest results
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
-  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,11 @@
     <sheet name="$3_payout_structure_week8" sheetId="11" r:id="rId10"/>
     <sheet name="$4_payout_structure_week10" sheetId="12" r:id="rId11"/>
     <sheet name="$27_payout_structure_week15_thu" sheetId="13" r:id="rId12"/>
+    <sheet name="NFL $1.5M FRONT FOUR Wk16" sheetId="14" r:id="rId13"/>
+    <sheet name="NFL $40K PLAY-ACTION Wk16" sheetId="15" r:id="rId14"/>
+    <sheet name="NFL $1.25M CHOP BLOCK Wk16" sheetId="16" r:id="rId15"/>
+    <sheet name="NFL $500K THREE ENTRY MAX Wk16" sheetId="17" r:id="rId16"/>
+    <sheet name="ASUALNFL$225KFLEAFLICKER Wk 16" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>1st</t>
   </si>
@@ -47,15 +52,6 @@
     <t>5th</t>
   </si>
   <si>
-    <t>6th</t>
-  </si>
-  <si>
-    <t>7th - 8th</t>
-  </si>
-  <si>
-    <t>9th - 10th</t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
@@ -68,34 +64,67 @@
     <t>Place_hi</t>
   </si>
   <si>
-    <t>11th - 13th</t>
+    <t>11th - 15th</t>
   </si>
   <si>
-    <t>14th - 18th</t>
+    <t>6th</t>
   </si>
   <si>
-    <t>19th - 25th</t>
+    <t>9th - 10th</t>
   </si>
   <si>
-    <t>26th - 37th</t>
+    <t>7th</t>
   </si>
   <si>
-    <t>38th - 65th</t>
+    <t>8th</t>
   </si>
   <si>
-    <t>66th - 115th</t>
+    <t>16th - 20th</t>
   </si>
   <si>
-    <t>116th - 190th</t>
+    <t>21st - 25th</t>
   </si>
   <si>
-    <t>191st - 305th</t>
+    <t>26th - 35th</t>
   </si>
   <si>
-    <t>306th - 465th</t>
+    <t>36th - 60th</t>
   </si>
   <si>
-    <t>466th - 752nd</t>
+    <t>61st - 85th</t>
+  </si>
+  <si>
+    <t>86th - 135th</t>
+  </si>
+  <si>
+    <t>136th - 200th</t>
+  </si>
+  <si>
+    <t>201st - 275th</t>
+  </si>
+  <si>
+    <t>276th - 375th</t>
+  </si>
+  <si>
+    <t>376th - 550th</t>
+  </si>
+  <si>
+    <t>551st - 900th</t>
+  </si>
+  <si>
+    <t>901st - 1550th</t>
+  </si>
+  <si>
+    <t>1551st - 2700th</t>
+  </si>
+  <si>
+    <t>2701st - 4950th</t>
+  </si>
+  <si>
+    <t>4951st - 8350th</t>
+  </si>
+  <si>
+    <t>8351st - 13725th</t>
   </si>
 </sst>
 </file>
@@ -148,8 +177,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -205,7 +246,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -226,6 +267,12 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -246,6 +293,12 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,7 +631,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="D1:F19"/>
+      <selection activeCell="F27" sqref="D1:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -592,19 +645,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -612,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -622,7 +675,7 @@
       </c>
       <c r="F2" s="3">
         <f>B2</f>
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -631,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:E7" si="0">D2+1</f>
@@ -643,7 +696,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F34" si="1">B3</f>
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -652,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -664,7 +717,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -673,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -685,7 +738,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -694,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -706,16 +759,16 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -727,91 +780,91 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>750</v>
-      </c>
-      <c r="D8" s="2" t="str">
+        <v>1250</v>
+      </c>
+      <c r="D8" s="2" t="e">
         <f t="shared" ref="D8:D34" si="2">LEFT(A8,FIND(" ",A8)-3)</f>
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E8" s="2" t="e">
         <f t="shared" ref="E8:E34" si="3">MID(A8,FIND(" ",A8)+3,FIND("t",A8,FIND("t",A8)+1)-(FIND(" ",A8)+3))</f>
-        <v>8</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>1250</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
-        <v>550</v>
-      </c>
-      <c r="D9" s="2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E9" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>750</v>
+      </c>
+      <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="str">
+      <c r="E10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>550</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1">
-        <v>400</v>
-      </c>
-      <c r="D10" s="2" t="str">
+        <v>750</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>600</v>
+      </c>
+      <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="E10" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1">
-        <v>300</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -820,19 +873,19 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -841,19 +894,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -862,19 +915,19 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -883,19 +936,19 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -904,19 +957,19 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>190</v>
+        <v>85</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -925,19 +978,19 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>305</v>
+        <v>135</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -946,19 +999,19 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>306</v>
+        <v>136</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>465</v>
+        <v>200</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -967,147 +1020,187 @@
         <v>21</v>
       </c>
       <c r="B19" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>466</v>
-      </c>
-      <c r="E19" s="2" t="e">
+        <v>201</v>
+      </c>
+      <c r="E19" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>275</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2" t="e">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="2" t="e">
+        <v>276</v>
+      </c>
+      <c r="E20" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>375</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2" t="e">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E21" s="2" t="e">
+        <v>376</v>
+      </c>
+      <c r="E21" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>550</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2" t="e">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E22" s="2" t="e">
+        <v>551</v>
+      </c>
+      <c r="E22" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>900</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="B23" s="1"/>
-      <c r="D23" s="2" t="e">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E23" s="2" t="e">
+        <v>901</v>
+      </c>
+      <c r="E23" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>1550</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="B24" s="1"/>
-      <c r="D24" s="2" t="e">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E24" s="2" t="e">
+        <v>1551</v>
+      </c>
+      <c r="E24" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>2700</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="B25" s="1"/>
-      <c r="D25" s="2" t="e">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E25" s="2" t="e">
+        <v>2701</v>
+      </c>
+      <c r="E25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>4950</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="B26" s="1"/>
-      <c r="D26" s="2" t="e">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E26" s="2" t="e">
+        <v>4951</v>
+      </c>
+      <c r="E26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>8350</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="B27" s="1"/>
-      <c r="D27" s="2" t="e">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E27" s="2" t="e">
+        <v>8351</v>
+      </c>
+      <c r="E27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>13725</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -1225,6 +1318,18 @@
     </row>
     <row r="35" spans="2:9">
       <c r="B35" s="1"/>
+      <c r="D35" s="2" t="e">
+        <f t="shared" ref="D35" si="4">LEFT(A35,FIND(" ",A35)-3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E35" s="2" t="e">
+        <f t="shared" ref="E35" si="5">MID(A35,FIND(" ",A35)+3,FIND("t",A35,FIND("t",A35)+1)-(FIND(" ",A35)+3))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" ref="F35" si="6">B35</f>
+        <v>0</v>
+      </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="2:9">
@@ -1266,13 +1371,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1660,13 +1765,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2024,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2032,13 +2137,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2237,6 +2342,1547 @@
       </c>
       <c r="C19">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>201</v>
+      </c>
+      <c r="B18" s="5">
+        <v>250</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>251</v>
+      </c>
+      <c r="B19" s="5">
+        <v>350</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>351</v>
+      </c>
+      <c r="B20" s="5">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>501</v>
+      </c>
+      <c r="B21" s="5">
+        <v>750</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>751</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>1001</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1501</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2000</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2001</v>
+      </c>
+      <c r="B25" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>3001</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4500</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>4501</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6500</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>6501</v>
+      </c>
+      <c r="B28" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>10001</v>
+      </c>
+      <c r="B29" s="5">
+        <v>15000</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5">
+        <v>15001</v>
+      </c>
+      <c r="B30" s="5">
+        <v>20000</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5">
+        <v>20001</v>
+      </c>
+      <c r="B31" s="5">
+        <v>27500</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5">
+        <v>27501</v>
+      </c>
+      <c r="B32" s="5">
+        <v>37500</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5">
+        <v>37501</v>
+      </c>
+      <c r="B33" s="5">
+        <v>55000</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5">
+        <v>55001</v>
+      </c>
+      <c r="B34" s="5">
+        <v>80000</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5">
+        <v>80001</v>
+      </c>
+      <c r="B35" s="5">
+        <v>115500</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>41</v>
+      </c>
+      <c r="B14" s="5">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>51</v>
+      </c>
+      <c r="B15" s="5">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5">
+        <v>80</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>81</v>
+      </c>
+      <c r="B17" s="5">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>101</v>
+      </c>
+      <c r="B18" s="5">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>151</v>
+      </c>
+      <c r="B19" s="5">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>201</v>
+      </c>
+      <c r="B20" s="5">
+        <v>300</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>301</v>
+      </c>
+      <c r="B21" s="5">
+        <v>500</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>501</v>
+      </c>
+      <c r="B22" s="5">
+        <v>800</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>801</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1300</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1301</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2300</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2301</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4395</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5">
+        <v>75</v>
+      </c>
+      <c r="C13">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>76</v>
+      </c>
+      <c r="B14" s="5">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>101</v>
+      </c>
+      <c r="B15" s="5">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>151</v>
+      </c>
+      <c r="B16" s="5">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>201</v>
+      </c>
+      <c r="B17" s="5">
+        <v>300</v>
+      </c>
+      <c r="C17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>301</v>
+      </c>
+      <c r="B18" s="5">
+        <v>500</v>
+      </c>
+      <c r="C18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>501</v>
+      </c>
+      <c r="B19" s="5">
+        <v>750</v>
+      </c>
+      <c r="C19">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>751</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1250</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>1251</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2250</v>
+      </c>
+      <c r="C21">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>2251</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3750</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>3751</v>
+      </c>
+      <c r="B23" s="5">
+        <v>6350</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A17:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5">
+        <v>75</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>76</v>
+      </c>
+      <c r="B14" s="5">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>101</v>
+      </c>
+      <c r="B15" s="5">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>151</v>
+      </c>
+      <c r="B16" s="5">
+        <v>250</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>251</v>
+      </c>
+      <c r="B17" s="5">
+        <v>450</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>451</v>
+      </c>
+      <c r="B18" s="5">
+        <v>750</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>751</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1450</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>1451</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2830</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>2831</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5430</v>
+      </c>
+      <c r="C21">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>86</v>
+      </c>
+      <c r="B17" s="5">
+        <v>135</v>
+      </c>
+      <c r="C17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>136</v>
+      </c>
+      <c r="B18" s="5">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>201</v>
+      </c>
+      <c r="B19" s="5">
+        <v>275</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>276</v>
+      </c>
+      <c r="B20" s="5">
+        <v>375</v>
+      </c>
+      <c r="C20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>376</v>
+      </c>
+      <c r="B21" s="5">
+        <v>550</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>551</v>
+      </c>
+      <c r="B22" s="5">
+        <v>900</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>901</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1550</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1551</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2700</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2701</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4950</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>4951</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8350</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>8351</v>
+      </c>
+      <c r="B27" s="5">
+        <v>13725</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2261,13 +3907,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2710,13 +4356,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3102,13 +4748,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3496,13 +5142,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3835,13 +5481,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4152,13 +5798,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4524,13 +6170,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4753,13 +6399,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
testing value wr sunday only
</commit_message>
<xml_diff>
--- a/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
+++ b/resultsAnalysis/data_warehouse/weekly_payout_structure/payout_structure_week.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="2680" yWindow="320" windowWidth="24720" windowHeight="15180" tabRatio="894" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="clean_data" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="NFL $1.25M CHOP BLOCK Wk16" sheetId="16" r:id="rId15"/>
     <sheet name="NFL $500K THREE ENTRY MAX Wk16" sheetId="17" r:id="rId16"/>
     <sheet name="ASUALNFL$225KFLEAFLICKER Wk 16" sheetId="18" r:id="rId17"/>
+    <sheet name="NFL $1.1M PLAY-ACTION Wk17" sheetId="19" r:id="rId18"/>
+    <sheet name="NFL $400K COVER FOUR 3MAX Wk17" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
   <si>
     <t>1st</t>
   </si>
@@ -73,58 +75,64 @@
     <t>9th - 10th</t>
   </si>
   <si>
-    <t>7th</t>
-  </si>
-  <si>
-    <t>8th</t>
-  </si>
-  <si>
-    <t>16th - 20th</t>
-  </si>
-  <si>
-    <t>21st - 25th</t>
-  </si>
-  <si>
     <t>26th - 35th</t>
   </si>
   <si>
-    <t>36th - 60th</t>
+    <t>7th - 8th</t>
   </si>
   <si>
-    <t>61st - 85th</t>
+    <t>16th - 25th</t>
   </si>
   <si>
-    <t>86th - 135th</t>
+    <t>36th - 50th</t>
   </si>
   <si>
-    <t>136th - 200th</t>
+    <t>51st - 75th</t>
   </si>
   <si>
-    <t>201st - 275th</t>
+    <t>76th - 100th</t>
   </si>
   <si>
-    <t>276th - 375th</t>
+    <t>101st - 150th</t>
   </si>
   <si>
-    <t>376th - 550th</t>
+    <t>151st - 200th</t>
   </si>
   <si>
-    <t>551st - 900th</t>
+    <t>501st - 750th</t>
   </si>
   <si>
-    <t>901st - 1550th</t>
+    <t>751st - 1000th</t>
   </si>
   <si>
-    <t>1551st - 2700th</t>
+    <t>1001st - 1500th</t>
   </si>
   <si>
-    <t>2701st - 4950th</t>
+    <t>201st - 300th</t>
   </si>
   <si>
-    <t>4951st - 8350th</t>
+    <t>301st - 400th</t>
   </si>
   <si>
-    <t>8351st - 13725th</t>
+    <t>401st - 500th</t>
+  </si>
+  <si>
+    <t>1501st - 2500th</t>
+  </si>
+  <si>
+    <t>2501st - 4000th</t>
+  </si>
+  <si>
+    <t>4001st - 6500th</t>
+  </si>
+  <si>
+    <t>6501st - 11500th</t>
+  </si>
+  <si>
+    <t>11501st - 19000th</t>
+  </si>
+  <si>
+    <t>19001st - 28750th</t>
   </si>
 </sst>
 </file>
@@ -177,8 +185,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -246,7 +262,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +289,10 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -299,6 +319,10 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,7 +655,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="D1:F27"/>
+      <selection activeCell="D29" sqref="D1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -665,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -675,7 +699,7 @@
       </c>
       <c r="F2" s="3">
         <f>B2</f>
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -684,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:E7" si="0">D2+1</f>
@@ -696,7 +720,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F34" si="1">B3</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -705,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -717,7 +741,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -726,7 +750,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -738,7 +762,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -747,7 +771,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -759,7 +783,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -768,7 +792,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>1500</v>
+        <v>5000</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -780,108 +804,108 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>5000</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>1250</v>
-      </c>
-      <c r="D8" s="2" t="e">
+        <v>3500</v>
+      </c>
+      <c r="D8" s="2" t="str">
         <f t="shared" ref="D8:D34" si="2">LEFT(A8,FIND(" ",A8)-3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E8" s="2" t="e">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="str">
         <f t="shared" ref="E8:E34" si="3">MID(A8,FIND(" ",A8)+3,FIND("t",A8,FIND("t",A8)+1)-(FIND(" ",A8)+3))</f>
-        <v>#VALUE!</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>3500</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D9" s="2" t="e">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E9" s="2" t="e">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>500</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
@@ -894,19 +918,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -915,19 +939,19 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -940,11 +964,11 @@
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
@@ -957,19 +981,19 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -978,141 +1002,141 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>201</v>
+        <v>301</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>275</v>
+        <v>400</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>276</v>
+        <v>401</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>375</v>
+        <v>500</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>501</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>550</v>
+        <v>750</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>551</v>
+        <v>751</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>20</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>901</v>
+        <v>1001</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>1550</v>
+        <v>1500</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
@@ -1129,11 +1153,11 @@
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1551</v>
+        <v>1501</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>2500</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
@@ -1150,11 +1174,11 @@
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>2701</v>
+        <v>2501</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>4950</v>
+        <v>4000</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
@@ -1171,11 +1195,11 @@
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>4951</v>
+        <v>4001</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>8350</v>
+        <v>6500</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
@@ -1192,11 +1216,11 @@
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>8351</v>
+        <v>6501</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>13725</v>
+        <v>11500</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
@@ -1205,34 +1229,44 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="B28" s="1"/>
-      <c r="D28" s="2" t="e">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E28" s="2" t="e">
+        <v>11501</v>
+      </c>
+      <c r="E28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>19000</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="B29" s="1"/>
-      <c r="D29" s="2" t="e">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E29" s="2" t="e">
+        <v>19001</v>
+      </c>
+      <c r="E29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>28750</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -3582,7 +3616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -3883,6 +3917,736 @@
       </c>
       <c r="C27">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>201</v>
+      </c>
+      <c r="B18" s="5">
+        <v>250</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>251</v>
+      </c>
+      <c r="B19" s="5">
+        <v>350</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>351</v>
+      </c>
+      <c r="B20" s="5">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>501</v>
+      </c>
+      <c r="B21" s="5">
+        <v>750</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>751</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>1001</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1501</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2250</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2251</v>
+      </c>
+      <c r="B25" s="5">
+        <v>3250</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>3251</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4750</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>4751</v>
+      </c>
+      <c r="B27" s="5">
+        <v>7000</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>7001</v>
+      </c>
+      <c r="B28" s="5">
+        <v>11000</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>11001</v>
+      </c>
+      <c r="B29" s="5">
+        <v>17000</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5">
+        <v>17001</v>
+      </c>
+      <c r="B30" s="5">
+        <v>25000</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5">
+        <v>25001</v>
+      </c>
+      <c r="B31" s="5">
+        <v>35000</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5">
+        <v>35001</v>
+      </c>
+      <c r="B32" s="5">
+        <v>50000</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5">
+        <v>50001</v>
+      </c>
+      <c r="B33" s="5">
+        <v>75000</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5">
+        <v>75001</v>
+      </c>
+      <c r="B34" s="5">
+        <v>119450</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5">
+        <v>101</v>
+      </c>
+      <c r="B16" s="5">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5">
+        <v>201</v>
+      </c>
+      <c r="B18" s="5">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5">
+        <v>301</v>
+      </c>
+      <c r="B19" s="5">
+        <v>400</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5">
+        <v>401</v>
+      </c>
+      <c r="B20" s="5">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5">
+        <v>501</v>
+      </c>
+      <c r="B21" s="5">
+        <v>750</v>
+      </c>
+      <c r="C21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5">
+        <v>751</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5">
+        <v>1001</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>1501</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5">
+        <v>2501</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5">
+        <v>4001</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6500</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5">
+        <v>6501</v>
+      </c>
+      <c r="B27" s="5">
+        <v>11500</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>11501</v>
+      </c>
+      <c r="B28" s="5">
+        <v>19000</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>19001</v>
+      </c>
+      <c r="B29" s="5">
+        <v>28750</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>